<commit_message>
Spreadsheet refactoring + Cunha
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22415" windowHeight="12362"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22415" windowHeight="12362" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Smells" sheetId="1" r:id="rId1"/>
+    <sheet name="Refactorings" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Refactorings!$B$1:$H$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Smells!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>LabVIEW/G</t>
   </si>
@@ -277,13 +279,79 @@
   </si>
   <si>
     <t>Unreferenced data cell*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Empty Cell (amind nonempty cells)- Cunha</t>
+  </si>
+  <si>
+    <t>Pattern finder (inconsistent cell) - Cunha</t>
+  </si>
+  <si>
+    <t>Standard Devation - Cunha</t>
+  </si>
+  <si>
+    <t>String distance - Cunha</t>
+  </si>
+  <si>
+    <t>Default value (null, 0, "")</t>
+  </si>
+  <si>
+    <t>Reference to empty cell - Cunha</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Extract method</t>
+  </si>
+  <si>
+    <t>Extract VI (part of other VI)</t>
+  </si>
+  <si>
+    <t>Extract subformula</t>
+  </si>
+  <si>
+    <t>Add/Remove Parameter</t>
+  </si>
+  <si>
+    <t>Add/Remove terminal in block diagram</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Extract literal</t>
+  </si>
+  <si>
+    <t>Define named constant</t>
+  </si>
+  <si>
+    <t>Extract subformula / Extract row or column</t>
+  </si>
+  <si>
+    <t>Quasi-functional dependencies - Cunha</t>
+  </si>
+  <si>
+    <t>Make cell constant / Make references absolute - Badame</t>
+  </si>
+  <si>
+    <t>Guard Call / prevent divide by zero - Badame</t>
+  </si>
+  <si>
+    <t>Replace awkward formula - Badame</t>
+  </si>
+  <si>
+    <t>String to dropdown - Badame</t>
+  </si>
+  <si>
+    <t>Introduce cell name - Badame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +381,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -368,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -422,6 +498,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +803,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -718,30 +815,36 @@
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" style="23" customWidth="1"/>
+    <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -754,12 +857,12 @@
       <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -770,12 +873,12 @@
       <c r="D3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -786,12 +889,12 @@
       <c r="D4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -802,12 +905,12 @@
       <c r="D5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -818,8 +921,12 @@
       <c r="D6" s="19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="24">
+        <f>Refactorings!A4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -831,7 +938,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -843,7 +950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -853,7 +960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -865,7 +972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
@@ -875,7 +982,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -885,7 +992,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -894,8 +1001,12 @@
       <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="24">
+        <f>Refactorings!A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -905,7 +1016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -915,7 +1026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1064,68 +1175,216 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="20" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Processed feedback. Moved Cunha & Barowy to related work. Incorporated Sui in refactoring LabVIEW.
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22415" windowHeight="12362" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22415" windowHeight="10732"/>
   </bookViews>
   <sheets>
     <sheet name="Smells" sheetId="1" r:id="rId1"/>
@@ -332,12 +332,6 @@
     <t>Quasi-functional dependencies - Cunha</t>
   </si>
   <si>
-    <t>Make cell constant / Make references absolute - Badame</t>
-  </si>
-  <si>
-    <t>Guard Call / prevent divide by zero - Badame</t>
-  </si>
-  <si>
     <t>Replace awkward formula - Badame</t>
   </si>
   <si>
@@ -345,6 +339,12 @@
   </si>
   <si>
     <t>Introduce cell name - Badame</t>
+  </si>
+  <si>
+    <t>Make cell constant (=Make references absolute) - Badame</t>
+  </si>
+  <si>
+    <t>Guard Call (prevent divide by zero) - Badame</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1264,8 +1264,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1353,28 +1353,43 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="E5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small modifications & TODO's as a result of conference call.
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
   <si>
     <t>LabVIEW/G</t>
   </si>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>Extract VI (part of other VI)</t>
-  </si>
-  <si>
-    <t>Extract subformula</t>
   </si>
   <si>
     <t>Add/Remove Parameter</t>
@@ -806,7 +803,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A31" sqref="A31:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1175,24 +1172,14 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="21" t="s">
-        <v>80</v>
-      </c>
+      <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
@@ -1241,7 +1228,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,7 +1239,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1280,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>3</v>
@@ -1313,7 +1300,7 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="14" t="s">
@@ -1325,10 +1312,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1342,10 +1329,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="14" t="s">
@@ -1357,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,7 +1352,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1373,7 +1360,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1381,7 +1368,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1389,7 +1376,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added two more YP smells to table
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\git\end_user_refactoring\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22415" windowHeight="10732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19080"/>
   </bookViews>
   <sheets>
     <sheet name="Smells" sheetId="1" r:id="rId1"/>
@@ -19,8 +14,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Refactorings!$B$1:$H$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Smells!$A$1:$H$42</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -34,7 +32,7 @@
     <author>David</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
   <si>
     <t>LabVIEW/G</t>
   </si>
@@ -342,6 +340,12 @@
   </si>
   <si>
     <t>Guard Call (prevent divide by zero) - Badame</t>
+  </si>
+  <si>
+    <t>Unfamiliar Constructs*</t>
+  </si>
+  <si>
+    <t>Excessive abstraction*</t>
   </si>
 </sst>
 </file>
@@ -577,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -789,7 +793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -797,27 +801,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:D32"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" style="23" customWidth="1"/>
-    <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
@@ -841,7 +845,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -859,7 +863,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="28">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -875,7 +879,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -891,7 +895,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -907,7 +911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -923,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -935,7 +939,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -947,7 +951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -957,7 +961,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -969,7 +973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
@@ -979,7 +983,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -989,7 +993,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1003,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1023,7 +1027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1033,17 +1037,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1063,7 +1069,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
@@ -1073,7 +1079,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1083,7 +1089,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
@@ -1091,7 +1097,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1113,7 +1119,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1123,7 +1129,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>21</v>
@@ -1131,7 +1137,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1141,7 +1147,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
         <v>14</v>
       </c>
@@ -1151,7 +1157,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -1161,7 +1167,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="28">
       <c r="A30" s="12" t="s">
         <v>69</v>
       </c>
@@ -1171,19 +1177,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1191,7 +1197,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1199,7 +1205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1207,7 +1213,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1215,7 +1221,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="21" t="s">
         <v>75</v>
       </c>
@@ -1225,13 +1231,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1"/>
       <c r="D38" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
+      <c r="C39" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1239,14 +1250,19 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="69" orientation="landscape"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H41"/>
@@ -1255,17 +1271,17 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="25" t="s">
         <v>82</v>
       </c>
@@ -1288,7 +1304,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1307,7 +1323,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1324,7 +1340,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1339,7 +1355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1347,7 +1363,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1355,7 +1371,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1363,7 +1379,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1371,7 +1387,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1379,7 +1395,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -1387,6 +1403,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Spreadsheet specific smells, Excel screenshot
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\git\end_user_refactoring\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27900" windowHeight="19080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27903" windowHeight="19087"/>
   </bookViews>
   <sheets>
     <sheet name="Smells" sheetId="1" r:id="rId1"/>
@@ -14,13 +19,13 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Refactorings!$B$1:$H$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Smells!$A$1:$H$42</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -32,7 +37,7 @@
     <author>David</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>LabVIEW/G</t>
   </si>
@@ -346,6 +351,9 @@
   </si>
   <si>
     <t>Excessive abstraction*</t>
+  </si>
+  <si>
+    <t>Inconsistent Formula - Excel already</t>
   </si>
 </sst>
 </file>
@@ -793,7 +801,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -801,27 +809,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="23" customWidth="1"/>
+    <col min="8" max="8" width="38.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
@@ -845,7 +853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -863,7 +871,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28">
+    <row r="3" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -879,7 +887,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
@@ -895,7 +903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -911,7 +919,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -927,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -939,7 +947,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>64</v>
       </c>
@@ -951,7 +959,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -961,7 +969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -973,7 +981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>42</v>
       </c>
@@ -983,7 +991,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>67</v>
       </c>
@@ -993,7 +1001,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>29</v>
       </c>
@@ -1007,7 +1015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1059,7 +1067,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1069,7 +1077,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
@@ -1079,7 +1087,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="28">
+    <row r="21" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1089,7 +1097,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
@@ -1097,7 +1105,7 @@
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1119,7 +1127,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1129,7 +1137,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>21</v>
@@ -1137,7 +1145,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
@@ -1147,7 +1155,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>14</v>
       </c>
@@ -1157,7 +1165,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>16</v>
       </c>
@@ -1167,7 +1175,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="28">
+    <row r="30" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>69</v>
       </c>
@@ -1177,19 +1185,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="21"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1197,7 +1205,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1205,7 +1213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1213,7 +1221,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1221,7 +1229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
         <v>75</v>
       </c>
@@ -1231,18 +1239,23 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="D38" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C39" s="16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1262,7 +1275,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H41"/>
@@ -1271,17 +1284,17 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>82</v>
       </c>
@@ -1304,7 +1317,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1323,7 +1336,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1340,7 +1353,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1355,7 +1368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1363,7 +1376,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1371,7 +1384,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1379,7 +1392,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1387,7 +1400,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1395,7 +1408,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>

</xml_diff>

<commit_message>
added lego mindstorms to the story
</commit_message>
<xml_diff>
--- a/smell comparison.xlsx
+++ b/smell comparison.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\git\end_user_refactoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felienne\Dropbox\TU Delft\Papers\end_user_refactoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27903" windowHeight="19087" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="Smells" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>David:</t>
         </r>
@@ -54,7 +54,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 I don't fully understand the difference between these two smells</t>
@@ -385,14 +385,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -820,19 +820,19 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1181,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>69</v>
       </c>
@@ -1286,18 +1286,18 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>